<commit_message>
unhcr data analysis (cool insights)
</commit_message>
<xml_diff>
--- a/converting_UA_codes.xlsx
+++ b/converting_UA_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/econ390/project-git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA711B46-41F3-0A47-A96B-922214C83FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB05193C-59F7-5544-8AD7-4973F6E9A4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="500" windowWidth="16460" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12340" yWindow="500" windowWidth="16460" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,21 +49,9 @@
     <t>Chernihivska oblast</t>
   </si>
   <si>
-    <t>UA-77</t>
-  </si>
-  <si>
-    <t>UA77</t>
-  </si>
-  <si>
     <t>Chernivetska oblast</t>
   </si>
   <si>
-    <t>UA-43</t>
-  </si>
-  <si>
-    <t>UA43</t>
-  </si>
-  <si>
     <t>Avtonomna Respublika Krym</t>
   </si>
   <si>
@@ -124,12 +112,6 @@
     <t>Khmelnytska oblast</t>
   </si>
   <si>
-    <t>UA-30</t>
-  </si>
-  <si>
-    <t>UA30</t>
-  </si>
-  <si>
     <t>Kyiv</t>
   </si>
   <si>
@@ -163,12 +145,6 @@
     <t>Lvivska oblast</t>
   </si>
   <si>
-    <t>UA-09</t>
-  </si>
-  <si>
-    <t>UA09</t>
-  </si>
-  <si>
     <t>Luhanska oblast</t>
   </si>
   <si>
@@ -208,12 +184,6 @@
     <t>Rivnenska oblast</t>
   </si>
   <si>
-    <t>UA-40</t>
-  </si>
-  <si>
-    <t>UA40</t>
-  </si>
-  <si>
     <t>Sevastopol</t>
   </si>
   <si>
@@ -355,9 +325,6 @@
     <t>Ternopil'</t>
   </si>
   <si>
-    <t>Transcarpathia</t>
-  </si>
-  <si>
     <t>Vinnytsya</t>
   </si>
   <si>
@@ -368,6 +335,39 @@
   </si>
   <si>
     <t>Zhytomyr</t>
+  </si>
+  <si>
+    <t>UA-80</t>
+  </si>
+  <si>
+    <t>UA80</t>
+  </si>
+  <si>
+    <t>UA-85</t>
+  </si>
+  <si>
+    <t>UA85</t>
+  </si>
+  <si>
+    <t>Zakarpatska</t>
+  </si>
+  <si>
+    <t>UA-01</t>
+  </si>
+  <si>
+    <t>UA01</t>
+  </si>
+  <si>
+    <t>UA-73</t>
+  </si>
+  <si>
+    <t>UA73</t>
+  </si>
+  <si>
+    <t>UA-44</t>
+  </si>
+  <si>
+    <t>UA44</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -670,13 +670,13 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -751,16 +751,16 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>5</v>
@@ -772,19 +772,19 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -793,16 +793,16 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
@@ -814,16 +814,16 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -835,16 +835,16 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
@@ -856,16 +856,16 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
@@ -877,16 +877,16 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
@@ -898,16 +898,16 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
@@ -919,19 +919,19 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -940,16 +940,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
@@ -961,16 +961,16 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>5</v>
@@ -982,16 +982,16 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>5</v>
@@ -1003,16 +1003,16 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>5</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>5</v>
@@ -1045,16 +1045,16 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
@@ -1066,16 +1066,16 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>5</v>
@@ -1087,16 +1087,16 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
@@ -1108,19 +1108,19 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1129,16 +1129,16 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>5</v>
@@ -1150,16 +1150,16 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>5</v>
@@ -1171,16 +1171,16 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>5</v>
@@ -1192,16 +1192,16 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>5</v>
@@ -1213,16 +1213,16 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>5</v>
@@ -1234,16 +1234,16 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>5</v>
@@ -1255,16 +1255,16 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>5</v>

</xml_diff>